<commit_message>
Added R and S measurement pictures
</commit_message>
<xml_diff>
--- a/MeetingFiles/FilesForMeeting_5_6_2020/Measurement/CV- curves/SMV1249_CapVsReverseVoltage.xlsx
+++ b/MeetingFiles/FilesForMeeting_5_6_2020/Measurement/CV- curves/SMV1249_CapVsReverseVoltage.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\Capstone_Rohde-Schwarz_Team13\Measurements\Capacitance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\Capstone_Rohde-Schwarz_Team13\MeetingFiles\FilesForMeeting_5_6_2020\Measurement\CV- curves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BD54486-F33C-46FA-90C3-71DF10A63B2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C3DCFB2-0994-47B1-89BA-87F0493DD313}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="-120" windowWidth="37590" windowHeight="16440" xr2:uid="{831434E3-B5F5-4249-9DF3-A9C46302E0FC}"/>
+    <workbookView xWindow="38280" yWindow="-6810" windowWidth="16440" windowHeight="28440" xr2:uid="{831434E3-B5F5-4249-9DF3-A9C46302E0FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -491,8 +492,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1263,16 +1265,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>